<commit_message>
add all the stops in all lines
</commit_message>
<xml_diff>
--- a/cta_L_stops_new.xlsx
+++ b/cta_L_stops_new.xlsx
@@ -9,15 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29840" yWindow="-10980" windowWidth="26320" windowHeight="17360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="29840" yWindow="-10000" windowWidth="23900" windowHeight="17360" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cta_L_stops_new" sheetId="1" r:id="rId1"/>
-    <sheet name="orange" sheetId="6" r:id="rId2"/>
-    <sheet name="green" sheetId="5" r:id="rId3"/>
-    <sheet name="red" sheetId="2" r:id="rId4"/>
-    <sheet name="red (2)" sheetId="3" r:id="rId5"/>
-    <sheet name="blue" sheetId="4" r:id="rId6"/>
+    <sheet name="yellow" sheetId="9" r:id="rId2"/>
+    <sheet name="purple" sheetId="8" r:id="rId3"/>
+    <sheet name="brown" sheetId="7" r:id="rId4"/>
+    <sheet name="orange" sheetId="6" r:id="rId5"/>
+    <sheet name="green" sheetId="5" r:id="rId6"/>
+    <sheet name="red" sheetId="2" r:id="rId7"/>
+    <sheet name="red (2)" sheetId="3" r:id="rId8"/>
+    <sheet name="blue" sheetId="4" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cta_L_stops_new!$D$1:$Q$299</definedName>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2504" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2897" uniqueCount="735">
   <si>
     <t>STOP_ID</t>
   </si>
@@ -2225,6 +2228,21 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>custom list</t>
+  </si>
+  <si>
+    <t>custom output via template</t>
+  </si>
+  <si>
+    <t>http://www.convertcsv.com/csv-to-json.htm</t>
+  </si>
+  <si>
+    <t>South Blvd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     {h4}: {</t>
   </si>
 </sst>
 </file>
@@ -2581,7 +2599,7 @@
   <dimension ref="A1:Q299"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E294"/>
+      <selection activeCell="E233" sqref="A1:E233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2751,7 +2769,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -2804,7 +2822,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -4023,7 +4041,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -4659,7 +4677,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>116</v>
       </c>
@@ -4818,7 +4836,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>116</v>
       </c>
@@ -7309,7 +7327,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>229</v>
       </c>
@@ -8581,7 +8599,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="114" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>282</v>
       </c>
@@ -8634,7 +8652,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="115" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>282</v>
       </c>
@@ -10012,7 +10030,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>342</v>
       </c>
@@ -10118,7 +10136,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>342</v>
       </c>
@@ -10542,7 +10560,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>365</v>
       </c>
@@ -10754,7 +10772,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="155" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>375</v>
       </c>
@@ -10807,7 +10825,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="156" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>375</v>
       </c>
@@ -11814,7 +11832,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>419</v>
       </c>
@@ -11867,7 +11885,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>419</v>
       </c>
@@ -12980,7 +12998,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>469</v>
       </c>
@@ -13669,7 +13687,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>504</v>
       </c>
@@ -13722,7 +13740,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>504</v>
       </c>
@@ -14835,7 +14853,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="232" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>556</v>
       </c>
@@ -14888,7 +14906,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="233" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>556</v>
       </c>
@@ -15312,7 +15330,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>576</v>
       </c>
@@ -15365,7 +15383,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>576</v>
       </c>
@@ -15683,7 +15701,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>592</v>
       </c>
@@ -16107,7 +16125,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>612</v>
       </c>
@@ -16160,7 +16178,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>612</v>
       </c>
@@ -17114,7 +17132,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>652</v>
       </c>
@@ -17538,7 +17556,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="283" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>672</v>
       </c>
@@ -17591,7 +17609,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="284" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>677</v>
       </c>
@@ -18068,7 +18086,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="293" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>687</v>
       </c>
@@ -18121,7 +18139,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="294" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>687</v>
       </c>
@@ -18441,7 +18459,7 @@
     </row>
   </sheetData>
   <autoFilter ref="D1:Q299">
-    <filterColumn colId="12">
+    <filterColumn colId="10">
       <filters>
         <filter val="TRUE"/>
       </filters>
@@ -18453,10 +18471,1984 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection sqref="A1:D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B2">
+        <v>40140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>30026</v>
+      </c>
+      <c r="E2" t="s">
+        <v>281</v>
+      </c>
+      <c r="I2" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B3">
+        <v>40140</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <v>30027</v>
+      </c>
+      <c r="E3" t="s">
+        <v>285</v>
+      </c>
+      <c r="I3" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B4">
+        <v>41680</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>30298</v>
+      </c>
+      <c r="E4" t="s">
+        <v>555</v>
+      </c>
+      <c r="I4" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>556</v>
+      </c>
+      <c r="B5">
+        <v>41680</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>30297</v>
+      </c>
+      <c r="E5" t="s">
+        <v>559</v>
+      </c>
+      <c r="I5" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>375</v>
+      </c>
+      <c r="B6">
+        <v>40900</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>30176</v>
+      </c>
+      <c r="E6" t="s">
+        <v>374</v>
+      </c>
+      <c r="I6" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>375</v>
+      </c>
+      <c r="B7">
+        <v>40900</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>30175</v>
+      </c>
+      <c r="E7" t="s">
+        <v>378</v>
+      </c>
+      <c r="I7" t="s">
+        <v>726</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>479</v>
+      </c>
+      <c r="B2">
+        <v>41050</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>30203</v>
+      </c>
+      <c r="E2" t="s">
+        <v>478</v>
+      </c>
+      <c r="J2" t="s">
+        <v>730</v>
+      </c>
+      <c r="M2" t="s">
+        <v>731</v>
+      </c>
+      <c r="P2" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B3">
+        <v>41050</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <v>30204</v>
+      </c>
+      <c r="E3" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4">
+        <v>41250</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>30242</v>
+      </c>
+      <c r="E4" t="s">
+        <v>173</v>
+      </c>
+      <c r="J4" t="s">
+        <v>479</v>
+      </c>
+      <c r="M4" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5">
+        <v>41250</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>30241</v>
+      </c>
+      <c r="E5" t="s">
+        <v>177</v>
+      </c>
+      <c r="J5" t="s">
+        <v>174</v>
+      </c>
+      <c r="M5" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>542</v>
+      </c>
+      <c r="B6">
+        <v>40400</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>30079</v>
+      </c>
+      <c r="E6" t="s">
+        <v>541</v>
+      </c>
+      <c r="J6" t="s">
+        <v>542</v>
+      </c>
+      <c r="M6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>542</v>
+      </c>
+      <c r="B7">
+        <v>40400</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>30078</v>
+      </c>
+      <c r="E7" t="s">
+        <v>545</v>
+      </c>
+      <c r="J7" t="s">
+        <v>302</v>
+      </c>
+      <c r="M7" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>302</v>
+      </c>
+      <c r="B8">
+        <v>40520</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>30101</v>
+      </c>
+      <c r="E8" t="s">
+        <v>301</v>
+      </c>
+      <c r="J8" t="s">
+        <v>272</v>
+      </c>
+      <c r="M8" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>302</v>
+      </c>
+      <c r="B9">
+        <v>40520</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9">
+        <v>30102</v>
+      </c>
+      <c r="E9" t="s">
+        <v>305</v>
+      </c>
+      <c r="J9" t="s">
+        <v>277</v>
+      </c>
+      <c r="M9" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>272</v>
+      </c>
+      <c r="B10">
+        <v>40050</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>30010</v>
+      </c>
+      <c r="E10" t="s">
+        <v>271</v>
+      </c>
+      <c r="J10" t="s">
+        <v>494</v>
+      </c>
+      <c r="M10" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>272</v>
+      </c>
+      <c r="B11">
+        <v>40050</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11">
+        <v>30011</v>
+      </c>
+      <c r="E11" t="s">
+        <v>275</v>
+      </c>
+      <c r="J11" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B12">
+        <v>40690</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12">
+        <v>30133</v>
+      </c>
+      <c r="E12" t="s">
+        <v>276</v>
+      </c>
+      <c r="J12" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>277</v>
+      </c>
+      <c r="B13">
+        <v>40690</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13">
+        <v>30134</v>
+      </c>
+      <c r="E13" t="s">
+        <v>280</v>
+      </c>
+      <c r="J13" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>494</v>
+      </c>
+      <c r="B14">
+        <v>40270</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14">
+        <v>30052</v>
+      </c>
+      <c r="E14" t="s">
+        <v>493</v>
+      </c>
+      <c r="J14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>494</v>
+      </c>
+      <c r="B15">
+        <v>40270</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15">
+        <v>30053</v>
+      </c>
+      <c r="E15" t="s">
+        <v>497</v>
+      </c>
+      <c r="J15" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>733</v>
+      </c>
+      <c r="B16">
+        <v>40840</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>30163</v>
+      </c>
+      <c r="E16" t="s">
+        <v>636</v>
+      </c>
+      <c r="J16" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>733</v>
+      </c>
+      <c r="B17">
+        <v>40840</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17">
+        <v>30164</v>
+      </c>
+      <c r="E17" t="s">
+        <v>640</v>
+      </c>
+      <c r="J17" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>375</v>
+      </c>
+      <c r="B18">
+        <v>40900</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18">
+        <v>30176</v>
+      </c>
+      <c r="E18" t="s">
+        <v>374</v>
+      </c>
+      <c r="J18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>375</v>
+      </c>
+      <c r="B19">
+        <v>40900</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19">
+        <v>30175</v>
+      </c>
+      <c r="E19" t="s">
+        <v>378</v>
+      </c>
+      <c r="J19" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>706</v>
+      </c>
+      <c r="B20">
+        <v>40540</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20">
+        <v>30106</v>
+      </c>
+      <c r="E20" t="s">
+        <v>705</v>
+      </c>
+      <c r="J20" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>706</v>
+      </c>
+      <c r="B21">
+        <v>40540</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21">
+        <v>30105</v>
+      </c>
+      <c r="E21" t="s">
+        <v>709</v>
+      </c>
+      <c r="J21" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22">
+        <v>41320</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22">
+        <v>30258</v>
+      </c>
+      <c r="E22" t="s">
+        <v>138</v>
+      </c>
+      <c r="J22" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23">
+        <v>41320</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23">
+        <v>30257</v>
+      </c>
+      <c r="E23" t="s">
+        <v>148</v>
+      </c>
+      <c r="J23" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>682</v>
+      </c>
+      <c r="B24">
+        <v>41210</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24">
+        <v>30231</v>
+      </c>
+      <c r="E24" t="s">
+        <v>681</v>
+      </c>
+      <c r="J24" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>682</v>
+      </c>
+      <c r="B25">
+        <v>41210</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25">
+        <v>30232</v>
+      </c>
+      <c r="E25" t="s">
+        <v>685</v>
+      </c>
+      <c r="J25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>287</v>
+      </c>
+      <c r="B26">
+        <v>40530</v>
+      </c>
+      <c r="C26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26">
+        <v>30103</v>
+      </c>
+      <c r="E26" t="s">
+        <v>286</v>
+      </c>
+      <c r="J26" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>287</v>
+      </c>
+      <c r="B27">
+        <v>40530</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27">
+        <v>30104</v>
+      </c>
+      <c r="E27" t="s">
+        <v>290</v>
+      </c>
+      <c r="J27" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>312</v>
+      </c>
+      <c r="B28">
+        <v>41220</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28">
+        <v>30236</v>
+      </c>
+      <c r="E28" t="s">
+        <v>315</v>
+      </c>
+      <c r="J28" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>312</v>
+      </c>
+      <c r="B29">
+        <v>41220</v>
+      </c>
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29">
+        <v>30235</v>
+      </c>
+      <c r="E29" t="s">
+        <v>316</v>
+      </c>
+      <c r="J29" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30">
+        <v>40660</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <v>30128</v>
+      </c>
+      <c r="E30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31">
+        <v>40660</v>
+      </c>
+      <c r="C31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31">
+        <v>30127</v>
+      </c>
+      <c r="E31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>625</v>
+      </c>
+      <c r="B32">
+        <v>40800</v>
+      </c>
+      <c r="C32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32">
+        <v>30155</v>
+      </c>
+      <c r="E32" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>625</v>
+      </c>
+      <c r="B33">
+        <v>40800</v>
+      </c>
+      <c r="C33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33">
+        <v>30156</v>
+      </c>
+      <c r="E33" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>198</v>
+      </c>
+      <c r="B34">
+        <v>40710</v>
+      </c>
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34">
+        <v>30138</v>
+      </c>
+      <c r="E34" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>198</v>
+      </c>
+      <c r="B35">
+        <v>40710</v>
+      </c>
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35">
+        <v>30137</v>
+      </c>
+      <c r="E35" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>499</v>
+      </c>
+      <c r="B36">
+        <v>40460</v>
+      </c>
+      <c r="C36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36">
+        <v>30091</v>
+      </c>
+      <c r="E36" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>499</v>
+      </c>
+      <c r="B37">
+        <v>40460</v>
+      </c>
+      <c r="C37" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37">
+        <v>30090</v>
+      </c>
+      <c r="E37" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>229</v>
+      </c>
+      <c r="B38">
+        <v>40380</v>
+      </c>
+      <c r="C38" t="s">
+        <v>729</v>
+      </c>
+      <c r="D38">
+        <v>30074</v>
+      </c>
+      <c r="E38" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>652</v>
+      </c>
+      <c r="B39">
+        <v>40260</v>
+      </c>
+      <c r="C39" t="s">
+        <v>729</v>
+      </c>
+      <c r="D39">
+        <v>30050</v>
+      </c>
+      <c r="E39" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>672</v>
+      </c>
+      <c r="B40">
+        <v>41700</v>
+      </c>
+      <c r="C40" t="s">
+        <v>729</v>
+      </c>
+      <c r="D40">
+        <v>30384</v>
+      </c>
+      <c r="E40" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41">
+        <v>40680</v>
+      </c>
+      <c r="C41" t="s">
+        <v>729</v>
+      </c>
+      <c r="D41">
+        <v>30132</v>
+      </c>
+      <c r="E41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>728</v>
+      </c>
+      <c r="B42">
+        <v>40850</v>
+      </c>
+      <c r="C42" t="s">
+        <v>729</v>
+      </c>
+      <c r="D42">
+        <v>30166</v>
+      </c>
+      <c r="E42" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>469</v>
+      </c>
+      <c r="B43">
+        <v>40160</v>
+      </c>
+      <c r="C43" t="s">
+        <v>729</v>
+      </c>
+      <c r="D43">
+        <v>30031</v>
+      </c>
+      <c r="E43" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>592</v>
+      </c>
+      <c r="B44">
+        <v>40040</v>
+      </c>
+      <c r="C44" t="s">
+        <v>729</v>
+      </c>
+      <c r="D44">
+        <v>30007</v>
+      </c>
+      <c r="E44" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>677</v>
+      </c>
+      <c r="B45">
+        <v>40730</v>
+      </c>
+      <c r="C45" t="s">
+        <v>729</v>
+      </c>
+      <c r="D45">
+        <v>30141</v>
+      </c>
+      <c r="E45" t="s">
+        <v>676</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:E45">
+    <sortCondition ref="A2:A45" customList="Linden,Central,Noyes,Foster,Davis,Dempster,Main,South Blvd,Howard,Wilson,Belmont,Wellington,Diversey,Fullerton,Armitage,Sedgwick,Chicago,Merchandise Mart,Washington/Wells,Quincy/Wells,LaSalle/Van Buren,Harold Washington Library,Adams"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:Q10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>439</v>
+      </c>
+      <c r="B2">
+        <v>41290</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>30249</v>
+      </c>
+      <c r="E2" t="s">
+        <v>438</v>
+      </c>
+      <c r="J2" t="s">
+        <v>730</v>
+      </c>
+      <c r="N2" t="s">
+        <v>731</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>439</v>
+      </c>
+      <c r="B3">
+        <v>41290</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <v>30250</v>
+      </c>
+      <c r="E3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B4">
+        <v>41180</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>30226</v>
+      </c>
+      <c r="E4" t="s">
+        <v>418</v>
+      </c>
+      <c r="J4" t="s">
+        <v>439</v>
+      </c>
+      <c r="N4" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B5">
+        <v>41180</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>30225</v>
+      </c>
+      <c r="E5" t="s">
+        <v>428</v>
+      </c>
+      <c r="J5" t="s">
+        <v>419</v>
+      </c>
+      <c r="N5" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>307</v>
+      </c>
+      <c r="B6">
+        <v>40870</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>30168</v>
+      </c>
+      <c r="E6" t="s">
+        <v>306</v>
+      </c>
+      <c r="J6" t="s">
+        <v>307</v>
+      </c>
+      <c r="N6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>307</v>
+      </c>
+      <c r="B7">
+        <v>40870</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>30167</v>
+      </c>
+      <c r="E7" t="s">
+        <v>310</v>
+      </c>
+      <c r="J7" t="s">
+        <v>607</v>
+      </c>
+      <c r="N7" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>607</v>
+      </c>
+      <c r="B8">
+        <v>41010</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8">
+        <v>30196</v>
+      </c>
+      <c r="E8" t="s">
+        <v>606</v>
+      </c>
+      <c r="J8" t="s">
+        <v>687</v>
+      </c>
+      <c r="N8" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>607</v>
+      </c>
+      <c r="B9">
+        <v>41010</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>30195</v>
+      </c>
+      <c r="E9" t="s">
+        <v>610</v>
+      </c>
+      <c r="J9" t="s">
+        <v>260</v>
+      </c>
+      <c r="N9" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>687</v>
+      </c>
+      <c r="B10">
+        <v>41480</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10">
+        <v>30284</v>
+      </c>
+      <c r="E10" t="s">
+        <v>690</v>
+      </c>
+      <c r="J10" t="s">
+        <v>518</v>
+      </c>
+      <c r="N10" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>687</v>
+      </c>
+      <c r="B11">
+        <v>41480</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>30283</v>
+      </c>
+      <c r="E11" t="s">
+        <v>693</v>
+      </c>
+      <c r="J11" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>260</v>
+      </c>
+      <c r="B12">
+        <v>40090</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>30019</v>
+      </c>
+      <c r="E12" t="s">
+        <v>259</v>
+      </c>
+      <c r="J12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>260</v>
+      </c>
+      <c r="B13">
+        <v>40090</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>30018</v>
+      </c>
+      <c r="E13" t="s">
+        <v>270</v>
+      </c>
+      <c r="J13" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>518</v>
+      </c>
+      <c r="B14">
+        <v>41500</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14">
+        <v>30287</v>
+      </c>
+      <c r="E14" t="s">
+        <v>522</v>
+      </c>
+      <c r="J14" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>518</v>
+      </c>
+      <c r="B15">
+        <v>41500</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15">
+        <v>30288</v>
+      </c>
+      <c r="E15" t="s">
+        <v>525</v>
+      </c>
+      <c r="J15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>391</v>
+      </c>
+      <c r="B16">
+        <v>41460</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16">
+        <v>30282</v>
+      </c>
+      <c r="E16" t="s">
+        <v>390</v>
+      </c>
+      <c r="J16" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>391</v>
+      </c>
+      <c r="B17">
+        <v>41460</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17">
+        <v>30281</v>
+      </c>
+      <c r="E17" t="s">
+        <v>398</v>
+      </c>
+      <c r="J17" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18">
+        <v>41440</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18">
+        <v>30277</v>
+      </c>
+      <c r="E18" t="s">
+        <v>96</v>
+      </c>
+      <c r="J18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19">
+        <v>41440</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19">
+        <v>30278</v>
+      </c>
+      <c r="E19" t="s">
+        <v>102</v>
+      </c>
+      <c r="J19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>566</v>
+      </c>
+      <c r="B20">
+        <v>41310</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20">
+        <v>30254</v>
+      </c>
+      <c r="E20" t="s">
+        <v>565</v>
+      </c>
+      <c r="J20" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>566</v>
+      </c>
+      <c r="B21">
+        <v>41310</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21">
+        <v>30253</v>
+      </c>
+      <c r="E21" t="s">
+        <v>569</v>
+      </c>
+      <c r="J21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B22">
+        <v>40360</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22">
+        <v>30070</v>
+      </c>
+      <c r="E22" t="s">
+        <v>641</v>
+      </c>
+      <c r="J22" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>642</v>
+      </c>
+      <c r="B23">
+        <v>40360</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23">
+        <v>30071</v>
+      </c>
+      <c r="E23" t="s">
+        <v>645</v>
+      </c>
+      <c r="J23" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24">
+        <v>41320</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24">
+        <v>30258</v>
+      </c>
+      <c r="E24" t="s">
+        <v>138</v>
+      </c>
+      <c r="J24" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B25">
+        <v>41320</v>
+      </c>
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25">
+        <v>30257</v>
+      </c>
+      <c r="E25" t="s">
+        <v>148</v>
+      </c>
+      <c r="J25" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>682</v>
+      </c>
+      <c r="B26">
+        <v>41210</v>
+      </c>
+      <c r="C26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26">
+        <v>30231</v>
+      </c>
+      <c r="E26" t="s">
+        <v>681</v>
+      </c>
+      <c r="J26" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>682</v>
+      </c>
+      <c r="B27">
+        <v>41210</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27">
+        <v>30232</v>
+      </c>
+      <c r="E27" t="s">
+        <v>685</v>
+      </c>
+      <c r="J27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>287</v>
+      </c>
+      <c r="B28">
+        <v>40530</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28">
+        <v>30103</v>
+      </c>
+      <c r="E28" t="s">
+        <v>286</v>
+      </c>
+      <c r="J28" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>287</v>
+      </c>
+      <c r="B29">
+        <v>40530</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29">
+        <v>30104</v>
+      </c>
+      <c r="E29" t="s">
+        <v>290</v>
+      </c>
+      <c r="J29" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>312</v>
+      </c>
+      <c r="B30">
+        <v>41220</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <v>30236</v>
+      </c>
+      <c r="E30" t="s">
+        <v>315</v>
+      </c>
+      <c r="J30" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>312</v>
+      </c>
+      <c r="B31">
+        <v>41220</v>
+      </c>
+      <c r="C31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31">
+        <v>30235</v>
+      </c>
+      <c r="E31" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32">
+        <v>40660</v>
+      </c>
+      <c r="C32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32">
+        <v>30128</v>
+      </c>
+      <c r="E32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33">
+        <v>40660</v>
+      </c>
+      <c r="C33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33">
+        <v>30127</v>
+      </c>
+      <c r="E33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>625</v>
+      </c>
+      <c r="B34">
+        <v>40800</v>
+      </c>
+      <c r="C34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34">
+        <v>30155</v>
+      </c>
+      <c r="E34" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>625</v>
+      </c>
+      <c r="B35">
+        <v>40800</v>
+      </c>
+      <c r="C35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35">
+        <v>30156</v>
+      </c>
+      <c r="E35" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>198</v>
+      </c>
+      <c r="B36">
+        <v>40710</v>
+      </c>
+      <c r="C36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36">
+        <v>30138</v>
+      </c>
+      <c r="E36" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>198</v>
+      </c>
+      <c r="B37">
+        <v>40710</v>
+      </c>
+      <c r="C37" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37">
+        <v>30137</v>
+      </c>
+      <c r="E37" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>499</v>
+      </c>
+      <c r="B38">
+        <v>40460</v>
+      </c>
+      <c r="C38" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38">
+        <v>30091</v>
+      </c>
+      <c r="E38" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>499</v>
+      </c>
+      <c r="B39">
+        <v>40460</v>
+      </c>
+      <c r="C39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39">
+        <v>30090</v>
+      </c>
+      <c r="E39" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>677</v>
+      </c>
+      <c r="B40">
+        <v>40730</v>
+      </c>
+      <c r="C40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40">
+        <v>30142</v>
+      </c>
+      <c r="E40" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>592</v>
+      </c>
+      <c r="B41">
+        <v>40040</v>
+      </c>
+      <c r="C41" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41">
+        <v>30008</v>
+      </c>
+      <c r="E41" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>469</v>
+      </c>
+      <c r="B42">
+        <v>40160</v>
+      </c>
+      <c r="C42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42">
+        <v>30030</v>
+      </c>
+      <c r="E42" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>728</v>
+      </c>
+      <c r="B43">
+        <v>40850</v>
+      </c>
+      <c r="C43" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43">
+        <v>30165</v>
+      </c>
+      <c r="E43" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44">
+        <v>40680</v>
+      </c>
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44">
+        <v>30131</v>
+      </c>
+      <c r="E44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>672</v>
+      </c>
+      <c r="B45">
+        <v>41700</v>
+      </c>
+      <c r="C45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45">
+        <v>30383</v>
+      </c>
+      <c r="E45" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>652</v>
+      </c>
+      <c r="B46">
+        <v>40260</v>
+      </c>
+      <c r="C46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46">
+        <v>30051</v>
+      </c>
+      <c r="E46" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>229</v>
+      </c>
+      <c r="B47">
+        <v>40380</v>
+      </c>
+      <c r="C47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47">
+        <v>30075</v>
+      </c>
+      <c r="E47" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:F47">
+    <sortCondition ref="A2:A47" customList="Kimball,Kedzie,Francisco,Rockwell,Western,Damen,Montrose,Irving Park,Addison,Paulina,Southport,Belmont,Wellington,Diversey,Fullerton,Armitage,Sedgwick,Chicago,Merchandise Mart,Washington/Wells,Quincy/Wells,LaSalle/Van Buren,Harold Wa"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O25"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18464,7 +20456,7 @@
     <col min="3" max="3" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>711</v>
       </c>
@@ -18481,7 +20473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>504</v>
       </c>
@@ -18498,10 +20490,16 @@
         <v>503</v>
       </c>
       <c r="I2" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>730</v>
+      </c>
+      <c r="L2" t="s">
+        <v>731</v>
+      </c>
+      <c r="O2" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>504</v>
       </c>
@@ -18517,11 +20515,8 @@
       <c r="E3" t="s">
         <v>507</v>
       </c>
-      <c r="I3" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>576</v>
       </c>
@@ -18538,10 +20533,13 @@
         <v>575</v>
       </c>
       <c r="I4" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>504</v>
+      </c>
+      <c r="L4" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>576</v>
       </c>
@@ -18558,10 +20556,13 @@
         <v>581</v>
       </c>
       <c r="I5" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>576</v>
+      </c>
+      <c r="L5" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>419</v>
       </c>
@@ -18578,10 +20579,13 @@
         <v>418</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="L6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>419</v>
       </c>
@@ -18598,10 +20602,13 @@
         <v>424</v>
       </c>
       <c r="I7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>687</v>
+      </c>
+      <c r="L7" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>687</v>
       </c>
@@ -18618,10 +20625,13 @@
         <v>697</v>
       </c>
       <c r="I8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="L8" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>687</v>
       </c>
@@ -18638,10 +20648,13 @@
         <v>690</v>
       </c>
       <c r="I9" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="L9" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -18658,10 +20671,13 @@
         <v>25</v>
       </c>
       <c r="I10" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>342</v>
+      </c>
+      <c r="L10" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -18678,10 +20694,10 @@
         <v>30</v>
       </c>
       <c r="I11" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>116</v>
       </c>
@@ -18698,10 +20714,10 @@
         <v>115</v>
       </c>
       <c r="I12" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -18718,10 +20734,10 @@
         <v>123</v>
       </c>
       <c r="I13" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>342</v>
       </c>
@@ -18738,10 +20754,10 @@
         <v>345</v>
       </c>
       <c r="I14" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>342</v>
       </c>
@@ -18758,10 +20774,10 @@
         <v>349</v>
       </c>
       <c r="I15" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>612</v>
       </c>
@@ -18778,7 +20794,7 @@
         <v>611</v>
       </c>
       <c r="I16" t="s">
-        <v>672</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -18798,7 +20814,7 @@
         <v>615</v>
       </c>
       <c r="I17" t="s">
-        <v>88</v>
+        <v>652</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -18817,6 +20833,9 @@
       <c r="E18" t="s">
         <v>368</v>
       </c>
+      <c r="I18" t="s">
+        <v>672</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -18833,6 +20852,9 @@
       </c>
       <c r="E19" t="s">
         <v>472</v>
+      </c>
+      <c r="I19" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -18945,7 +20967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I61"/>
   <sheetViews>
@@ -19907,12 +21929,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I8" sqref="I2:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21288,7 +23310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J67"/>
   <sheetViews>
@@ -22758,7 +24780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J67"/>
   <sheetViews>

</xml_diff>